<commit_message>
Added projects for Kalendar and program for videos
</commit_message>
<xml_diff>
--- a/doc/arduino_switch.xlsx
+++ b/doc/arduino_switch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\3Dsimo\Boffin\Podklady\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2252F6AD-0FFA-4BF8-873B-812F908F3607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF8278F-792E-439B-AC9F-A7ED2C4BEA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{61B28506-4AB0-4F8D-BCE2-F6D556376503}"/>
+    <workbookView xWindow="1950" yWindow="1125" windowWidth="11820" windowHeight="11385" xr2:uid="{61B28506-4AB0-4F8D-BCE2-F6D556376503}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Tetris</t>
   </si>
@@ -211,13 +211,31 @@
   </si>
   <si>
     <t>Volant</t>
+  </si>
+  <si>
+    <t>Songs</t>
+  </si>
+  <si>
+    <t>Hudba</t>
+  </si>
+  <si>
+    <t>Light Show</t>
+  </si>
+  <si>
+    <t>Světelná show</t>
+  </si>
+  <si>
+    <t>Vánoční hudba</t>
+  </si>
+  <si>
+    <t>Christmas song</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +250,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -396,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,9 +462,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -473,7 +498,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -771,11 +796,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7086A52C-CD1E-4780-96C9-C4F63B4F7843}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:L19"/>
+      <selection pane="bottomRight" activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,8 +3053,12 @@
       <c r="I66" s="4">
         <v>0</v>
       </c>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
+      <c r="J66" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="L66" s="10"/>
     </row>
     <row r="67" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3060,8 +3089,12 @@
       <c r="I67" s="4">
         <v>0</v>
       </c>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
+      <c r="J67" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K67" s="23" t="s">
+        <v>65</v>
+      </c>
       <c r="L67" s="10"/>
     </row>
     <row r="68" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3092,8 +3125,12 @@
       <c r="I68" s="4">
         <v>0</v>
       </c>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
+      <c r="J68" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="K68" s="23" t="s">
+        <v>66</v>
+      </c>
       <c r="L68" s="10"/>
     </row>
     <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>